<commit_message>
Added new client registration screens
</commit_message>
<xml_diff>
--- a/module_communication.xlsx
+++ b/module_communication.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsasala/Development/Aquarius New/aquarius-design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29FA915-6069-A846-B0A4-EE3C173DAE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F73345-37E5-9448-AEBC-360F2E266C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8220" yWindow="2260" windowWidth="37580" windowHeight="23700" activeTab="1" xr2:uid="{A0852067-D941-9F4F-8153-FAB53950511B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="133">
   <si>
     <t>Register Name</t>
   </si>
@@ -333,12 +333,6 @@
     <t>2 Bytes</t>
   </si>
   <si>
-    <t>Speed LSB</t>
-  </si>
-  <si>
-    <t>Speed MSB</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -396,34 +390,52 @@
     <t>0x3C</t>
   </si>
   <si>
-    <t>LSB (7::0)</t>
-  </si>
-  <si>
-    <t>MSB (15::8)</t>
-  </si>
-  <si>
     <t>2 bytes</t>
   </si>
   <si>
     <t>&lt;addr&gt;</t>
   </si>
   <si>
-    <t>Set Angle</t>
-  </si>
-  <si>
-    <t>Set Speed</t>
-  </si>
-  <si>
-    <t>Get Angle?</t>
-  </si>
-  <si>
-    <t>Get Speed?</t>
-  </si>
-  <si>
     <t>Function Addr</t>
   </si>
   <si>
     <t>Cmd Addr</t>
+  </si>
+  <si>
+    <t>Current - 0x30</t>
+  </si>
+  <si>
+    <t>Trigger Low</t>
+  </si>
+  <si>
+    <t>Trigger High</t>
+  </si>
+  <si>
+    <t>Angle (7::0)</t>
+  </si>
+  <si>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>Send Status</t>
+  </si>
+  <si>
+    <t>Pass/Fail</t>
+  </si>
+  <si>
+    <t>Receive Status</t>
+  </si>
+  <si>
+    <t>Buffer Size</t>
+  </si>
+  <si>
+    <t>Busy</t>
+  </si>
+  <si>
+    <t>True/False</t>
+  </si>
+  <si>
+    <t>Bulk</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1018,7 @@
         <v>71</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>77</v>
@@ -1026,7 +1038,7 @@
         <v>87</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>90</v>
@@ -1046,7 +1058,7 @@
         <v>73</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>91</v>
@@ -1066,7 +1078,7 @@
         <v>88</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>75</v>
@@ -1086,7 +1098,7 @@
         <v>89</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I7" s="4"/>
     </row>
@@ -1102,7 +1114,7 @@
       </c>
       <c r="F8" s="4"/>
       <c r="H8" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I8" s="4"/>
     </row>
@@ -1118,7 +1130,7 @@
       </c>
       <c r="F9" s="4"/>
       <c r="H9" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I9" s="4"/>
     </row>
@@ -1134,7 +1146,7 @@
       </c>
       <c r="F10" s="4"/>
       <c r="H10" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I10" s="4"/>
     </row>
@@ -1150,7 +1162,7 @@
       </c>
       <c r="F11" s="4"/>
       <c r="H11" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I11" s="4"/>
     </row>
@@ -1166,7 +1178,7 @@
       </c>
       <c r="F12" s="4"/>
       <c r="H12" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I12" s="4"/>
     </row>
@@ -1182,7 +1194,7 @@
       </c>
       <c r="F13" s="4"/>
       <c r="H13" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I13" s="4"/>
     </row>
@@ -1198,7 +1210,7 @@
       </c>
       <c r="F14" s="4"/>
       <c r="H14" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I14" s="4"/>
     </row>
@@ -1214,7 +1226,7 @@
       </c>
       <c r="F15" s="6"/>
       <c r="H15" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I15" s="6"/>
     </row>
@@ -1225,10 +1237,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D56ADDAB-025F-FE45-8D94-257C628CF870}">
-  <dimension ref="C2:R35"/>
+  <dimension ref="C2:R45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -1253,10 +1265,10 @@
   <sheetData>
     <row r="2" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C2" s="7" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>0</v>
@@ -1276,12 +1288,8 @@
       <c r="L2" s="15"/>
       <c r="M2" s="15"/>
       <c r="N2" s="9"/>
-      <c r="Q2" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>71</v>
-      </c>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="11"/>
     </row>
     <row r="3" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D3" s="15" t="s">
@@ -1311,12 +1319,8 @@
       <c r="N3" s="7">
         <v>6</v>
       </c>
-      <c r="Q3" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="R3" s="11" t="s">
-        <v>87</v>
-      </c>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="11"/>
     </row>
     <row r="4" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C4" s="12" t="s">
@@ -1347,12 +1351,8 @@
       <c r="L4" s="14"/>
       <c r="M4" s="14"/>
       <c r="N4" s="14"/>
-      <c r="Q4" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="R4" s="11" t="s">
-        <v>73</v>
-      </c>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="11"/>
     </row>
     <row r="5" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C5" s="12" t="s">
@@ -1389,12 +1389,8 @@
         <v>20</v>
       </c>
       <c r="N5" s="12"/>
-      <c r="Q5" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>88</v>
-      </c>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="11"/>
     </row>
     <row r="6" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C6" s="12" t="s">
@@ -1431,12 +1427,8 @@
         <v>25</v>
       </c>
       <c r="N6" s="12"/>
-      <c r="Q6" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="R6" s="11" t="s">
-        <v>89</v>
-      </c>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="11"/>
     </row>
     <row r="7" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C7" s="12" t="s">
@@ -1473,12 +1465,8 @@
         <v>28</v>
       </c>
       <c r="N7" s="12"/>
-      <c r="Q7" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="R7" s="11" t="s">
-        <v>77</v>
-      </c>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="11"/>
     </row>
     <row r="8" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C8" s="12" t="s">
@@ -1507,12 +1495,8 @@
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
       <c r="N8" s="14"/>
-      <c r="Q8" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="R8" s="11" t="s">
-        <v>90</v>
-      </c>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="11"/>
     </row>
     <row r="9" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D9" s="15" t="s">
@@ -1538,12 +1522,8 @@
       <c r="N9" s="7">
         <v>6</v>
       </c>
-      <c r="Q9" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="R9" s="11" t="s">
-        <v>91</v>
-      </c>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="11"/>
     </row>
     <row r="10" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C10" s="12" t="s">
@@ -1578,12 +1558,8 @@
       </c>
       <c r="M10" s="14"/>
       <c r="N10" s="14"/>
-      <c r="Q10" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="R10" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="11"/>
     </row>
     <row r="11" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C11" s="12" t="s">
@@ -1678,7 +1654,7 @@
         <v>46</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="J14" s="12" t="s">
         <v>45</v>
@@ -1747,13 +1723,13 @@
         <v>3</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>70</v>
@@ -1765,11 +1741,9 @@
         <v>95</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="L20" s="12" t="s">
-        <v>119</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="L20" s="12"/>
       <c r="M20" s="14"/>
       <c r="N20" s="12"/>
     </row>
@@ -1781,13 +1755,13 @@
         <v>7</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="H21" s="12" t="s">
         <v>70</v>
@@ -1799,69 +1773,35 @@
         <v>95</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="L21" s="12" t="s">
-        <v>98</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="L21" s="12"/>
       <c r="M21" s="12"/>
       <c r="N21" s="12"/>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C22" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="I22" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J22" s="12" t="s">
-        <v>95</v>
-      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
       <c r="N22" s="12"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C23" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="I23" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J23" s="12" t="s">
-        <v>95</v>
-      </c>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
@@ -1968,7 +1908,7 @@
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D29" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
@@ -1999,7 +1939,7 @@
         <v>3</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>97</v>
@@ -2010,18 +1950,44 @@
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="K30" s="12" t="s">
-        <v>100</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="K30" s="12"/>
       <c r="L30" s="12"/>
       <c r="M30" s="14"/>
       <c r="N30" s="14"/>
     </row>
+    <row r="31" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C31" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="K31" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="L31" s="12"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+    </row>
     <row r="33" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D33" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E33" s="15"/>
       <c r="F33" s="15"/>
@@ -2052,7 +2018,7 @@
         <v>3</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>97</v>
@@ -2060,10 +2026,14 @@
       <c r="G34" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
+      <c r="H34" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>3</v>
+      </c>
       <c r="J34" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K34" s="12" t="s">
         <v>45</v>
@@ -2080,7 +2050,7 @@
         <v>7</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="F35" s="12" t="s">
         <v>97</v>
@@ -2088,20 +2058,198 @@
       <c r="G35" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
+      <c r="H35" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>7</v>
+      </c>
       <c r="J35" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K35" s="12" t="s">
-        <v>45</v>
+        <v>127</v>
       </c>
       <c r="L35" s="12"/>
       <c r="M35" s="14"/>
       <c r="N35" s="14"/>
     </row>
+    <row r="36" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C36" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J36" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="K36" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="L36" s="12"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+    </row>
+    <row r="37" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C37" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J37" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="K37" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="L37" s="12"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+    </row>
+    <row r="42" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="D42" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="7">
+        <v>2</v>
+      </c>
+      <c r="K42" s="7">
+        <v>3</v>
+      </c>
+      <c r="L42" s="7">
+        <v>4</v>
+      </c>
+      <c r="M42" s="7">
+        <v>5</v>
+      </c>
+      <c r="N42" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C43" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="K43" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="L43" s="12"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="14"/>
+    </row>
+    <row r="44" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C44" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="K44" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="L44" s="12"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="14"/>
+    </row>
+    <row r="45" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C45" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="K45" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="L45" s="12"/>
+      <c r="M45" s="14"/>
+      <c r="N45" s="14"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="D42:G42"/>
     <mergeCell ref="D25:G25"/>
     <mergeCell ref="D29:G29"/>
     <mergeCell ref="D33:G33"/>

</xml_diff>